<commit_message>
Novas classes beans pro report
</commit_message>
<xml_diff>
--- a/documentacao/prototipos/etapa2/Luana/Relatorios.xlsx
+++ b/documentacao/prototipos/etapa2/Luana/Relatorios.xlsx
@@ -1,17 +1,18 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="45" windowWidth="20730" windowHeight="10035" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="2445" windowWidth="11055" windowHeight="4485" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Perfil Usuario" sheetId="1" r:id="rId1"/>
     <sheet name="Alimentacao" sheetId="2" r:id="rId2"/>
     <sheet name="Atividades" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="144525"/>
+  <calcPr calcId="0"/>
+  <oleSize ref="A4:G15"/>
 </workbook>
 </file>
 
@@ -600,63 +601,63 @@
   <dxfs count="21">
     <dxf>
       <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
         <b val="0"/>
         <i val="0"/>
         <strike val="0"/>
         <condense val="0"/>
         <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
         <outline val="0"/>
         <shadow val="0"/>
         <u val="none"/>
@@ -1068,17 +1069,17 @@
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Tabela2" displayName="Tabela2" ref="A14:D17" headerRowCount="0" totalsRowShown="0" headerRowDxfId="20" dataDxfId="19">
   <tableColumns count="4">
-    <tableColumn id="1" name="Colunas1" dataDxfId="16"/>
-    <tableColumn id="2" name="Colunas2" dataDxfId="15"/>
-    <tableColumn id="3" name="Colunas3" dataDxfId="14"/>
-    <tableColumn id="4" name="Colunas4" dataDxfId="13"/>
+    <tableColumn id="1" name="Colunas1" dataDxfId="18"/>
+    <tableColumn id="2" name="Colunas2" dataDxfId="17"/>
+    <tableColumn id="3" name="Colunas3" dataDxfId="16"/>
+    <tableColumn id="4" name="Colunas4" dataDxfId="15"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight21" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Tabela24" displayName="Tabela24" ref="A24:D27" headerRowCount="0" totalsRowShown="0" headerRowDxfId="18" dataDxfId="17">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Tabela24" displayName="Tabela24" ref="A24:D27" headerRowCount="0" totalsRowShown="0" headerRowDxfId="14" dataDxfId="13">
   <tableColumns count="4">
     <tableColumn id="1" name="Colunas1" dataDxfId="12"/>
     <tableColumn id="2" name="Colunas2" dataDxfId="11"/>
@@ -1094,10 +1095,10 @@
   <tableColumns count="6">
     <tableColumn id="1" name="Colunas1" dataDxfId="6"/>
     <tableColumn id="2" name="Colunas2" dataDxfId="5"/>
-    <tableColumn id="12" name="Colunas6" dataDxfId="0"/>
-    <tableColumn id="3" name="Colunas3" dataDxfId="4"/>
-    <tableColumn id="4" name="Colunas4" dataDxfId="3"/>
-    <tableColumn id="10" name="Colunas5" headerRowDxfId="1" dataDxfId="2"/>
+    <tableColumn id="12" name="Colunas6" dataDxfId="4"/>
+    <tableColumn id="3" name="Colunas3" dataDxfId="3"/>
+    <tableColumn id="4" name="Colunas4" dataDxfId="2"/>
+    <tableColumn id="10" name="Colunas5" headerRowDxfId="1" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight21" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1392,8 +1393,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:H26"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H21" sqref="H21"/>
+    <sheetView topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="A18" sqref="A18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1527,7 +1528,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:F30"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
       <selection activeCell="C20" sqref="C20"/>
     </sheetView>
   </sheetViews>
@@ -1769,7 +1770,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:F13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B21" sqref="B21"/>
     </sheetView>
   </sheetViews>

</xml_diff>